<commit_message>
barcodes ozon worked version
</commit_message>
<xml_diff>
--- a/tamplates/delivery_tamplate.xlsx
+++ b/tamplates/delivery_tamplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo-Projects\BEST-Delivery\tamplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADE263D-3BB0-456F-A8F5-0CA2C3C8BBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABE0D3E-9D97-4502-83F9-83CF304FB9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -259,7 +259,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -275,7 +275,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -285,21 +285,36 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thick">
@@ -311,8 +326,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -321,60 +338,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -656,18 +619,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -676,22 +635,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -700,88 +656,88 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1064,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,229 +1033,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="16">
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="11">
         <v>24</v>
       </c>
-      <c r="E1" s="17">
+      <c r="E1" s="12">
         <v>25</v>
       </c>
-      <c r="F1" s="17">
+      <c r="F1" s="12">
         <v>26</v>
       </c>
-      <c r="G1" s="17">
+      <c r="G1" s="12">
         <v>27</v>
       </c>
-      <c r="H1" s="17">
+      <c r="H1" s="12">
         <v>28</v>
       </c>
-      <c r="I1" s="17">
+      <c r="I1" s="12">
         <v>29</v>
       </c>
-      <c r="J1" s="17">
+      <c r="J1" s="12">
         <v>30</v>
       </c>
-      <c r="K1" s="17">
+      <c r="K1" s="12">
         <v>31</v>
       </c>
-      <c r="L1" s="17">
+      <c r="L1" s="12">
         <v>32</v>
       </c>
-      <c r="M1" s="17">
+      <c r="M1" s="12">
         <v>33</v>
       </c>
-      <c r="N1" s="17">
+      <c r="N1" s="12">
         <v>34</v>
       </c>
-      <c r="O1" s="18">
+      <c r="O1" s="13">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="21">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="16">
         <v>34</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="17">
         <v>35</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="17">
         <v>36</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="17">
         <v>37</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="17">
         <v>38</v>
       </c>
-      <c r="I2" s="22">
+      <c r="I2" s="17">
         <v>39</v>
       </c>
-      <c r="J2" s="22">
+      <c r="J2" s="17">
         <v>40</v>
       </c>
-      <c r="K2" s="22">
+      <c r="K2" s="17">
         <v>41</v>
       </c>
-      <c r="L2" s="23">
+      <c r="L2" s="18">
         <v>42</v>
       </c>
-      <c r="M2" s="23">
+      <c r="M2" s="18">
         <v>43</v>
       </c>
-      <c r="N2" s="23">
+      <c r="N2" s="18">
         <v>44</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="19">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="19">
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="14">
         <v>41</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="10">
         <v>42</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="10">
         <v>43</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="10">
         <v>44</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="10">
         <v>45</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="10">
         <v>46</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="10">
         <v>47</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="15">
         <v>48</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="46"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="41"/>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="36"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="31"/>
     </row>
-    <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="12">
+    <row r="5" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="8">
         <f>SUM(D5:O5)</f>
         <v>0</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="6"/>
     </row>
-    <row r="6" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="13">
-        <f>SUM(D6:O6)</f>
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="21">
+        <f>SUM(B5:B5)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="4"/>
+      <c r="C6" s="22">
+        <f>SUM(C5:C5)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36">
+        <f>SUM(B19/20)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="33"/>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="26">
-        <f>SUM(B5:B6)</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="27">
-        <f>SUM(C5:C6)</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="41">
-        <f>SUM(B20/20)</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="O7" s="38"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="D4:O4"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:M7"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:M6"/>
     <mergeCell ref="L3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: create excel deliveries witn привязка, заказ
</commit_message>
<xml_diff>
--- a/tamplates/delivery_tamplate.xlsx
+++ b/tamplates/delivery_tamplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo-Projects\BEST-Delivery\tamplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABE0D3E-9D97-4502-83F9-83CF304FB9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8E5252-C5A2-4004-BB34-D282DF3A5A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -371,21 +371,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -611,6 +596,19 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -619,14 +617,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -635,18 +633,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -656,12 +654,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -680,9 +678,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -701,44 +696,50 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1023,7 +1024,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,11 +1034,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
       <c r="D1" s="11">
         <v>24</v>
       </c>
@@ -1076,9 +1077,9 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="16">
         <v>34</v>
       </c>
@@ -1117,9 +1118,9 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="14">
         <v>41</v>
       </c>
@@ -1144,12 +1145,12 @@
       <c r="K3" s="15">
         <v>48</v>
       </c>
-      <c r="L3" s="39" t="s">
+      <c r="L3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="41"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="40"/>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
@@ -1161,28 +1162,25 @@
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="31"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="30"/>
     </row>
     <row r="5" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="8">
-        <f>SUM(D5:O5)</f>
-        <v>0</v>
-      </c>
+      <c r="C5" s="8"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -1204,29 +1202,29 @@
         <f>SUM(B5:B5)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="41">
         <f>SUM(C5:C5)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36">
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="35">
         <f>SUM(B19/20)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="32" t="s">
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="33"/>
+      <c r="O6" s="32"/>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>